<commit_message>
Added Edshultshall and Hälleviksstrand. Set place labels to be bold to differentiate from towns
</commit_message>
<xml_diff>
--- a/Data/Coordinates_Tjörn_v2.xlsx
+++ b/Data/Coordinates_Tjörn_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f7dd912bb4abd67/Sweden_Maps/DagsGifs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f7dd912bb4abd67/Sweden_Shipping_Maps/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AC870482-691A-474B-8972-196CE7977695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1D4D1F4-1B75-4D83-B21E-537D6A64A012}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{AC870482-691A-474B-8972-196CE7977695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{754DDD80-3443-4761-A1B9-791361B42BBF}"/>
   <bookViews>
-    <workbookView xWindow="1098" yWindow="870" windowWidth="15900" windowHeight="9330" xr2:uid="{E9969099-1D00-44CC-A3B0-4CC8D1287388}"/>
+    <workbookView xWindow="1464" yWindow="870" windowWidth="15900" windowHeight="9330" xr2:uid="{E9969099-1D00-44CC-A3B0-4CC8D1287388}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="63">
   <si>
     <t>Tjörn</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Skagerrak</t>
+  </si>
+  <si>
+    <t>Edshultshall</t>
+  </si>
+  <si>
+    <t>Hälleviksstrand</t>
   </si>
 </sst>
 </file>
@@ -585,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94369822-D42B-4189-B83F-B55F7B7DA12A}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1449,7 +1455,42 @@
         <v>8</v>
       </c>
     </row>
+    <row r="51" spans="2:6">
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>58.109400000000001</v>
+      </c>
+      <c r="E51">
+        <v>11.465299999999999</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>58.123800000000003</v>
+      </c>
+      <c r="E52">
+        <v>11.4435</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>